<commit_message>
Update analise of radio PKG
</commit_message>
<xml_diff>
--- a/app/src/main/res/doc/Analisys.xlsx
+++ b/app/src/main/res/doc/Analisys.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="20640" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20640" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Folder" sheetId="2" r:id="rId2"/>
-    <sheet name="Radio" sheetId="3" r:id="rId3"/>
+    <sheet name="Radio_new" sheetId="5" r:id="rId3"/>
     <sheet name="CRC" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="207">
   <si>
     <t>xx</t>
   </si>
@@ -367,96 +367,24 @@
     <t>183131</t>
   </si>
   <si>
-    <t>0F0A828896A9</t>
-  </si>
-  <si>
-    <t>0002</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
-    <t>- swithc fm2</t>
-  </si>
-  <si>
-    <t>87B28FA8CC0A</t>
-  </si>
-  <si>
-    <t>0001</t>
-  </si>
-  <si>
     <t>F4</t>
   </si>
   <si>
-    <t>- swithc fm1</t>
-  </si>
-  <si>
-    <t>000834617753</t>
-  </si>
-  <si>
-    <t>0011</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
-    <t>- switch Am</t>
-  </si>
-  <si>
     <t>FF50</t>
   </si>
   <si>
-    <t>1053</t>
-  </si>
-  <si>
     <t>FF40</t>
   </si>
   <si>
-    <t>4F</t>
-  </si>
-  <si>
-    <t>- 105.3 FM  Store2 (info)</t>
-  </si>
-  <si>
-    <t>1018</t>
-  </si>
-  <si>
-    <t>- 101.8 FM  Store3</t>
-  </si>
-  <si>
     <t>F890</t>
   </si>
   <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>Switch to</t>
-  </si>
-  <si>
-    <t>station type</t>
-  </si>
-  <si>
-    <t>F603</t>
-  </si>
-  <si>
-    <t>FF00</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>605 AM</t>
-  </si>
-  <si>
-    <t>store num</t>
-  </si>
-  <si>
-    <t xml:space="preserve">statuin </t>
-  </si>
-  <si>
-    <t>quality</t>
-  </si>
-  <si>
     <t>0101</t>
   </si>
   <si>
@@ -469,21 +397,6 @@
     <t>0400</t>
   </si>
   <si>
-    <t>1013</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>seek</t>
-  </si>
-  <si>
-    <t>0400 - seek +  0500 - seek -   0100 -Info          0110 - change station screen</t>
-  </si>
-  <si>
-    <t>station type    01 - FM1      02 - FM2     11 - AM</t>
-  </si>
-  <si>
     <t>684B31020300</t>
   </si>
   <si>
@@ -587,6 +500,144 @@
   </si>
   <si>
     <t>A1+</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>SrcDst</t>
+  </si>
+  <si>
+    <t>FM1</t>
+  </si>
+  <si>
+    <t>FM2</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>CommandId</t>
+  </si>
+  <si>
+    <t>Store ID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>Current play Radio Station</t>
+  </si>
+  <si>
+    <t>Active device</t>
+  </si>
+  <si>
+    <t>480D310302</t>
+  </si>
+  <si>
+    <t>4B00</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>0700</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>FM/CD</t>
+  </si>
+  <si>
+    <t>prepare to play</t>
+  </si>
+  <si>
+    <t>Playing</t>
+  </si>
+  <si>
+    <t>0102</t>
+  </si>
+  <si>
+    <t>FFFFFFFFFFFFFFFFFFFF</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>- STEREO</t>
+  </si>
+  <si>
+    <t>00000000000000000000</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>- BAD</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>1015</t>
+  </si>
+  <si>
+    <t>0500</t>
+  </si>
+  <si>
+    <t>1031</t>
+  </si>
+  <si>
+    <t>2F</t>
+  </si>
+  <si>
+    <t>SEEK</t>
+  </si>
+  <si>
+    <t>CommandID</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Right +</t>
+  </si>
+  <si>
+    <t>Left -</t>
+  </si>
+  <si>
+    <t>87B28FA8CC0A00</t>
+  </si>
+  <si>
+    <t>0F0A828896A900</t>
+  </si>
+  <si>
+    <t>00083461775300</t>
+  </si>
+  <si>
+    <t>Change to new Radio type</t>
+  </si>
+  <si>
+    <t>DATA(TODO: analisys)</t>
   </si>
 </sst>
 </file>
@@ -667,7 +718,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -758,11 +809,179 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -803,9 +1022,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -833,16 +1053,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -855,9 +1100,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -895,7 +1140,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -967,7 +1212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1169,26 +1414,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="32"/>
     </row>
     <row r="2" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -1427,57 +1672,57 @@
       <c r="R6" s="13"/>
     </row>
     <row r="7" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="23"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="26"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="23"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="26"/>
     </row>
     <row r="11" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1540,39 +1785,39 @@
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="26"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="29"/>
     </row>
     <row r="22" spans="1:13" s="11" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
@@ -2293,272 +2538,477 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" customWidth="1"/>
+    <col min="6" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="G1" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="50"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="41" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H5" s="41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="J6" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="K6" s="52"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="K7" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H16" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" s="46" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="I17" s="47" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="H18" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="20" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+    </row>
+    <row r="24" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="C24" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J6:K6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2566,7 +3016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2579,9 +3029,9 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -2604,49 +3054,49 @@
         <v>115</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>156</v>
+        <v>126</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>157</v>
+      <c r="E2" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="21" t="s">
         <v>60</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K2" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="K2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="31" t="s">
-        <v>159</v>
+      <c r="M2" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="O2" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="O2" s="21" t="s">
         <v>51</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -2654,49 +3104,49 @@
         <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>156</v>
+        <v>126</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>162</v>
+      <c r="E3" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="21" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="21" t="s">
         <v>60</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K3" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="K3" s="21" t="s">
         <v>3</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="31" t="s">
-        <v>159</v>
+      <c r="M3" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="O3" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="O3" s="21" t="s">
         <v>51</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -2704,49 +3154,49 @@
         <v>115</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>156</v>
+        <v>126</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>164</v>
+      <c r="E4" s="21" t="s">
+        <v>135</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="21" t="s">
         <v>60</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K4" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="K4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="31" t="s">
-        <v>159</v>
+      <c r="M4" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="O4" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="O4" s="21" t="s">
         <v>51</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -2754,49 +3204,49 @@
         <v>115</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>156</v>
+        <v>126</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>166</v>
+      <c r="E5" s="21" t="s">
+        <v>137</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="21" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="21" t="s">
         <v>60</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K5" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="K5" s="21" t="s">
         <v>3</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="31" t="s">
-        <v>159</v>
+      <c r="M5" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="O5" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="O5" s="21" t="s">
         <v>51</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -2804,49 +3254,49 @@
         <v>115</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>168</v>
+      <c r="E6" s="21" t="s">
+        <v>139</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="21" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="21" t="s">
         <v>60</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K6" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="K6" s="21" t="s">
         <v>3</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="31" t="s">
-        <v>169</v>
+      <c r="M6" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="O6" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="O6" s="21" t="s">
         <v>51</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -2854,46 +3304,46 @@
         <v>115</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>171</v>
+        <v>126</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>142</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>172</v>
+      <c r="E7" s="21" t="s">
+        <v>143</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="21" t="s">
         <v>60</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="21" t="s">
         <v>60</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K7" s="31" t="s">
-        <v>173</v>
+        <v>129</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>144</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="31" t="s">
+      <c r="M7" s="21" t="s">
         <v>90</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="O7" s="31" t="s">
-        <v>174</v>
+        <v>131</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>145</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>57</v>
@@ -2904,97 +3354,97 @@
         <v>115</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>171</v>
+        <v>126</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>142</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="31" t="s">
-        <v>172</v>
+      <c r="E8" s="21" t="s">
+        <v>143</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="21" t="s">
         <v>102</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="31" t="s">
-        <v>175</v>
+      <c r="I8" s="21" t="s">
+        <v>146</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="K8" s="31" t="s">
-        <v>173</v>
+        <v>129</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>144</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M8" s="21" t="s">
         <v>88</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="O8" s="31" t="s">
-        <v>174</v>
+        <v>131</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>145</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>178</v>
+      <c r="B9" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>149</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="31" t="s">
-        <v>179</v>
+      <c r="E9" s="21" t="s">
+        <v>150</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="31" t="s">
-        <v>178</v>
+      <c r="G9" s="21" t="s">
+        <v>149</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="31" t="s">
-        <v>178</v>
+      <c r="I9" s="21" t="s">
+        <v>149</v>
       </c>
       <c r="J9" s="3"/>
-      <c r="K9" s="31" t="s">
-        <v>178</v>
+      <c r="K9" s="21" t="s">
+        <v>149</v>
       </c>
       <c r="L9" s="3"/>
-      <c r="M9" s="31" t="s">
-        <v>178</v>
+      <c r="M9" s="21" t="s">
+        <v>149</v>
       </c>
       <c r="N9" s="3"/>
-      <c r="O9" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="P9" s="32" t="s">
+      <c r="O9" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="P9" s="22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="O10" s="30"/>
-    </row>
-    <row r="11" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="O10" s="20"/>
+    </row>
+    <row r="11" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>8</v>
       </c>
@@ -3005,68 +3455,68 @@
     </row>
     <row r="12" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>182</v>
+      <c r="C12" s="21" t="s">
+        <v>153</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>184</v>
+      <c r="C13" s="21" t="s">
+        <v>155</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="31" t="s">
-        <v>186</v>
+      <c r="C14" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>180</v>
+      <c r="B15" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C16" s="30"/>
+      <c r="C16" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added all track information
</commit_message>
<xml_diff>
--- a/app/src/main/res/doc/Analisys.xlsx
+++ b/app/src/main/res/doc/Analisys.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="20640" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20640" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CD Disk" sheetId="1" r:id="rId1"/>
     <sheet name="Folder" sheetId="2" r:id="rId2"/>
     <sheet name="Radio_new" sheetId="5" r:id="rId3"/>
     <sheet name="CRC" sheetId="4" r:id="rId4"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="276">
   <si>
     <t>xx</t>
   </si>
@@ -638,13 +638,220 @@
   </si>
   <si>
     <t>DATA(TODO: analisys)</t>
+  </si>
+  <si>
+    <t>00300036005F004F0061007300690073</t>
+  </si>
+  <si>
+    <t>005F004C00690076006500200046006F</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>00540068006500200057006F0072006C</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>Track name</t>
+  </si>
+  <si>
+    <t>0377</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>track#</t>
+  </si>
+  <si>
+    <t>pkg/all</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>folder#</t>
+  </si>
+  <si>
+    <t>subFolder#</t>
+  </si>
+  <si>
+    <t>sel/notSel</t>
+  </si>
+  <si>
+    <t>0370</t>
+  </si>
+  <si>
+    <t>0046006F006C0064006500720031FFFF</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>FFFFFFFFFFFFFFFFFFFFFFFFFFFFFFFF</t>
+  </si>
+  <si>
+    <t>6E</t>
+  </si>
+  <si>
+    <t>0371</t>
+  </si>
+  <si>
+    <t>00300038002E00200049006D006D0061</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>006E0065006E0074FFFFFFFFFFFFFFFF</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>0372</t>
+  </si>
+  <si>
+    <t>496D6D616E656E74FFFFFFFFFFFFFFFF</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>0374</t>
+  </si>
+  <si>
+    <t>4368696E65FFFFFFFFFFFFFFFFFFFFFF</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>0375</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>0376</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Folder NAME</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>Folder Name info</t>
+  </si>
+  <si>
+    <t>Src/Dst</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>fileCount</t>
+  </si>
+  <si>
+    <t>FilderID</t>
+  </si>
+  <si>
+    <t>CountFrom</t>
+  </si>
+  <si>
+    <t>0378</t>
+  </si>
+  <si>
+    <t>23720061006E006700650072002F005300</t>
+  </si>
+  <si>
+    <t>2361006C006B002000410062006F007500</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>22FFFFFFFFFFFFFFFFFFFFFFFFFFFFFFFF</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>FolderID</t>
+  </si>
+  <si>
+    <t>ParentFolderID</t>
+  </si>
+  <si>
+    <t>TrackNum</t>
+  </si>
+  <si>
+    <t>Active/No</t>
+  </si>
+  <si>
+    <t>TrackName</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Active Folder name</t>
+  </si>
+  <si>
+    <t>Active File name</t>
+  </si>
+  <si>
+    <t>Active Track name (Start first 2pkg)</t>
+  </si>
+  <si>
+    <t>End of 0372 command with Track location info (last paks)</t>
+  </si>
+  <si>
+    <t>0373</t>
+  </si>
+  <si>
+    <t>43006C006F007300750072006500FFFF</t>
+  </si>
+  <si>
+    <t>4D</t>
+  </si>
+  <si>
+    <t>Active Albome</t>
+  </si>
+  <si>
+    <t>Active Artist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -709,6 +916,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -981,7 +1196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1026,6 +1241,20 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1053,26 +1282,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1085,9 +1300,20 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1100,9 +1326,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1140,7 +1366,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1212,7 +1438,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1389,10 +1615,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R91"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,11 +1626,11 @@
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" customWidth="1"/>
     <col min="13" max="13" width="11.140625" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
@@ -1414,26 +1640,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="32"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="46"/>
     </row>
     <row r="2" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -1672,57 +1898,57 @@
       <c r="R6" s="13"/>
     </row>
     <row r="7" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="26"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="40"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="26"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="40"/>
     </row>
     <row r="11" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="43"/>
     </row>
     <row r="12" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1785,39 +2011,39 @@
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="29"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="43"/>
     </row>
     <row r="22" spans="1:13" s="11" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
@@ -2012,8 +2238,879 @@
         <v>57</v>
       </c>
     </row>
+    <row r="29" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+    </row>
+    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>223</v>
+      </c>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="H33" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="I33" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="J33" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="K33" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="48" t="s">
+        <v>267</v>
+      </c>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+    </row>
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="53" t="s">
+        <v>225</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="53" t="s">
+        <v>225</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="F40" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+    </row>
+    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>230</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="F45" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="48" t="s">
+        <v>269</v>
+      </c>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+    </row>
+    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="F50" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="G50" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="48" t="s">
+        <v>274</v>
+      </c>
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
+    </row>
+    <row r="53" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="33"/>
+      <c r="B55" s="33"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+    </row>
+    <row r="56" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="54"/>
+      <c r="B56" s="54"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="54"/>
+    </row>
+    <row r="57" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="54"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="54"/>
+    </row>
+    <row r="58" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="B58" s="48"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="48"/>
+    </row>
+    <row r="59" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="55"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="57"/>
+    </row>
+    <row r="64" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="B68" s="48"/>
+      <c r="C68" s="48"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="48"/>
+      <c r="H68" s="48"/>
+      <c r="I68" s="48"/>
+      <c r="J68" s="48"/>
+    </row>
+    <row r="69" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" s="53" t="s">
+        <v>245</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="53" t="s">
+        <v>245</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="B71" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="F71" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="G71" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="H71" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="I71" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="J71" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="48" t="s">
+        <v>270</v>
+      </c>
+      <c r="B74" s="48"/>
+      <c r="C74" s="48"/>
+      <c r="D74" s="48"/>
+      <c r="E74" s="48"/>
+      <c r="F74" s="48"/>
+      <c r="G74" s="48"/>
+      <c r="H74" s="48"/>
+      <c r="I74" s="48"/>
+      <c r="J74" s="48"/>
+      <c r="K74" s="48"/>
+      <c r="L74" s="48"/>
+    </row>
+    <row r="75" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K75" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="L75" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K77" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L77" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="33"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
+      <c r="E78" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="F78" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="G78" s="33"/>
+      <c r="H78" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="I78" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="J78" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="K78" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="L78" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="16">
+    <mergeCell ref="A29:K29"/>
+    <mergeCell ref="A68:J68"/>
+    <mergeCell ref="A74:L74"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A47:G47"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A63:G63"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A21:M21"/>
     <mergeCell ref="A1:R1"/>
@@ -2031,14 +3128,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2540,8 +3638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,13 +3655,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
       <c r="G1" s="49" t="s">
         <v>172</v>
       </c>
@@ -2585,16 +3683,16 @@
       <c r="E2" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="26" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2614,61 +3712,61 @@
       <c r="E3" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="30" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="28" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="30" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
       <c r="J6" s="51" t="s">
         <v>199</v>
       </c>
@@ -2699,10 +3797,10 @@
       <c r="H7" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="J7" s="36" t="s">
+      <c r="J7" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="26" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2731,47 +3829,47 @@
       <c r="H8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="K8" s="41" t="s">
+      <c r="K8" s="30" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="H9" s="44" t="s">
+      <c r="H9" s="33" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2786,10 +3884,10 @@
       <c r="D12" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="F12" s="46" t="s">
+      <c r="F12" s="35" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2806,24 +3904,24 @@
       <c r="D13" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="36" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -2847,10 +3945,10 @@
       <c r="G16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H16" s="45" t="s">
+      <c r="H16" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="I16" s="46" t="s">
+      <c r="I16" s="35" t="s">
         <v>200</v>
       </c>
     </row>
@@ -2876,48 +3974,48 @@
       <c r="G17" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H17" s="45" t="s">
+      <c r="H17" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="I17" s="47" t="s">
+      <c r="I17" s="36" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+    <row r="18" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="G18" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="H18" s="33" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+    <row r="20" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="47" t="s">
         <v>205</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -2979,33 +4077,33 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44" t="s">
+    <row r="24" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="33" t="s">
         <v>163</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3030,24 +4128,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3445,13 +4543,13 @@
       <c r="O10" s="20"/>
     </row>
     <row r="11" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">

</xml_diff>